<commit_message>
upd - added missing maps to dataset; new quarto doc for output.
</commit_message>
<xml_diff>
--- a/data/mw2022_tks.xlsx
+++ b/data/mw2022_tks.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MW/Desktop/Programming/R/Projects/2024-01_MWII_analysis/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C84994F-867C-B64B-B96F-F3CC38B2FDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet5" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="119">
   <si>
     <t>map</t>
   </si>
@@ -244,9 +253,6 @@
     <t>FireHead23</t>
   </si>
   <si>
-    <t>kunstenarr district</t>
-  </si>
-  <si>
     <t>Sigma Khan</t>
   </si>
   <si>
@@ -337,42 +343,79 @@
     <t>Dy_Smiling</t>
   </si>
   <si>
-    <t>koro</t>
-  </si>
-  <si>
     <t>shypie</t>
   </si>
   <si>
     <t>BigTedThe3rd-milk</t>
+  </si>
+  <si>
+    <t>embassy</t>
+  </si>
+  <si>
+    <t>Milky6</t>
+  </si>
+  <si>
+    <t>black gold</t>
+  </si>
+  <si>
+    <t>Twerk_Z</t>
+  </si>
+  <si>
+    <t>Chemicalz</t>
+  </si>
+  <si>
+    <t>punta mar</t>
+  </si>
+  <si>
+    <t>M40_bZ</t>
+  </si>
+  <si>
+    <t>himmelmatt</t>
+  </si>
+  <si>
+    <t>Yuladawg</t>
+  </si>
+  <si>
+    <t>kunstenarr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,48 +423,61 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -611,24 +667,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.0"/>
-    <col customWidth="1" min="4" max="4" width="17.88"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,12 +703,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>44868.0</v>
+        <v>44868</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -656,12 +717,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>44869.0</v>
+        <v>44869</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -670,12 +731,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>44869.0</v>
+        <v>44869</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -684,12 +745,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>44870.0</v>
+        <v>44870</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -698,12 +759,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>44870.0</v>
+        <v>44870</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -712,12 +773,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
-        <v>44870.0</v>
+        <v>44870</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -726,12 +787,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3">
-        <v>44871.0</v>
+        <v>44871</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -740,12 +801,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
-        <v>44878.0</v>
+        <v>44878</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -754,12 +815,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="3">
-        <v>44878.0</v>
+        <v>44878</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -768,12 +829,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3">
-        <v>44879.0</v>
+        <v>44879</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -782,12 +843,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3">
-        <v>44879.0</v>
+        <v>44879</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
@@ -796,12 +857,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="3">
-        <v>44996.0</v>
+        <v>44996</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
@@ -810,12 +871,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="3">
-        <v>44998.0</v>
+        <v>44998</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>8</v>
@@ -824,12 +885,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="3">
-        <v>44998.0</v>
+        <v>44998</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -838,12 +899,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="3">
-        <v>44998.0</v>
+        <v>44998</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -852,12 +913,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>44999.0</v>
+        <v>44999</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -866,12 +927,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="3">
-        <v>44999.0</v>
+        <v>44999</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -880,12 +941,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="3">
-        <v>44999.0</v>
+        <v>44999</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>5</v>
@@ -894,12 +955,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3">
-        <v>44999.0</v>
+        <v>44999</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -908,12 +969,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="3">
-        <v>44999.0</v>
+        <v>44999</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
@@ -922,12 +983,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3">
-        <v>44999.0</v>
+        <v>44999</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
@@ -936,12 +997,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="3">
-        <v>45000.0</v>
+        <v>45000</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
@@ -950,12 +1011,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="3">
-        <v>45001.0</v>
+        <v>45001</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -964,12 +1025,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="3">
-        <v>45001.0</v>
+        <v>45001</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
@@ -978,12 +1039,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="3">
-        <v>45001.0</v>
+        <v>45001</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -992,12 +1053,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="3">
-        <v>45002.0</v>
+        <v>45002</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1006,12 +1067,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="3">
-        <v>45005.0</v>
+        <v>45005</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>8</v>
@@ -1020,12 +1081,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="3">
-        <v>45005.0</v>
+        <v>45005</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>8</v>
@@ -1034,12 +1095,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="3">
-        <v>45005.0</v>
+        <v>45005</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
@@ -1048,12 +1109,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="3">
-        <v>45006.0</v>
+        <v>45006</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>5</v>
@@ -1062,12 +1123,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="3">
-        <v>45006.0</v>
+        <v>45006</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>5</v>
@@ -1076,12 +1137,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="3">
-        <v>45006.0</v>
+        <v>45006</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -1090,12 +1151,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="3">
-        <v>45006.0</v>
+        <v>45006</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>5</v>
@@ -1104,12 +1165,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B35" s="3">
-        <v>45007.0</v>
+        <v>45007</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>5</v>
@@ -1118,12 +1179,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="3">
-        <v>45007.0</v>
+        <v>45007</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>5</v>
@@ -1132,12 +1193,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="3">
-        <v>45008.0</v>
+        <v>45008</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>8</v>
@@ -1146,12 +1207,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="3">
-        <v>45014.0</v>
+        <v>45014</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>5</v>
@@ -1160,12 +1221,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="3">
-        <v>45016.0</v>
+        <v>45016</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>5</v>
@@ -1174,12 +1235,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="3">
-        <v>45016.0</v>
+        <v>45016</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>8</v>
@@ -1188,12 +1249,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="3">
-        <v>45017.0</v>
+        <v>45017</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>8</v>
@@ -1202,12 +1263,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="3">
-        <v>45017.0</v>
+        <v>45017</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>5</v>
@@ -1216,12 +1277,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="3">
-        <v>45018.0</v>
+        <v>45018</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>8</v>
@@ -1230,12 +1291,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B44" s="3">
-        <v>45018.0</v>
+        <v>45018</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>8</v>
@@ -1244,12 +1305,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="3">
-        <v>45018.0</v>
+        <v>45018</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>8</v>
@@ -1258,12 +1319,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B46" s="3">
-        <v>45018.0</v>
+        <v>45018</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
@@ -1272,12 +1333,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B47" s="3">
-        <v>45018.0</v>
+        <v>45018</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>8</v>
@@ -1286,12 +1347,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="3">
-        <v>45020.0</v>
+        <v>45020</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>8</v>
@@ -1300,12 +1361,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="3">
-        <v>45021.0</v>
+        <v>45021</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>8</v>
@@ -1314,12 +1375,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B50" s="3">
-        <v>45025.0</v>
+        <v>45025</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>5</v>
@@ -1328,12 +1389,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B51" s="3">
-        <v>45025.0</v>
+        <v>45025</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>5</v>
@@ -1342,12 +1403,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3">
-        <v>45025.0</v>
+        <v>45025</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>5</v>
@@ -1356,12 +1417,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="5">
-        <v>45025.0</v>
+        <v>45025</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>5</v>
@@ -1370,12 +1431,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="3">
-        <v>45025.0</v>
+        <v>45025</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>8</v>
@@ -1384,12 +1445,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B55" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>5</v>
@@ -1398,12 +1459,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B56" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>5</v>
@@ -1412,12 +1473,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>8</v>
@@ -1426,12 +1487,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B58" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>8</v>
@@ -1440,12 +1501,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B59" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>5</v>
@@ -1454,12 +1515,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B60" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>8</v>
@@ -1468,12 +1529,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B61" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>8</v>
@@ -1482,12 +1543,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B62" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>5</v>
@@ -1496,12 +1557,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B63" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>8</v>
@@ -1510,12 +1571,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B64" s="3">
-        <v>45026.0</v>
+        <v>45026</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>5</v>
@@ -1524,329 +1585,399 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A65" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="3">
+        <v>45230</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="3">
-        <v>45230.0</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66">
+    </row>
+    <row r="66" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B66" s="3">
-        <v>45231.0</v>
+        <v>45231</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2" t="s">
+      <c r="B67" s="3">
+        <v>45231</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="3">
-        <v>45231.0</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="2" t="s">
+    </row>
+    <row r="68" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A68" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="2" t="s">
+      <c r="B68" s="3">
+        <v>45232</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="3">
-        <v>45232.0</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="2" t="s">
+    </row>
+    <row r="69" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="2" t="s">
+      <c r="B69" s="3">
+        <v>45232</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B69" s="3">
-        <v>45232.0</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="2" t="s">
+    </row>
+    <row r="70" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A70" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="2" t="s">
+      <c r="B70" s="3">
+        <v>45232</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="3">
-        <v>45232.0</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="2" t="s">
+    </row>
+    <row r="71" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A71" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="3">
+        <v>45232</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="2" t="s">
+      <c r="B72" s="3">
+        <v>45233</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B71" s="3">
-        <v>45233.0</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="2" t="s">
+    </row>
+    <row r="73" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A73" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="2" t="s">
+      <c r="B73" s="3">
+        <v>45233</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B72" s="3">
-        <v>45233.0</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="2" t="s">
+    </row>
+    <row r="74" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="3">
+        <v>45233</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="3">
-        <v>45233.0</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="2" t="s">
+    <row r="75" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A75" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" s="3">
+        <v>45234</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B74" s="3">
-        <v>45234.0</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="2" t="s">
+    <row r="76" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A76" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="2" t="s">
+      <c r="B76" s="3">
+        <v>45234</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B75" s="3">
-        <v>45234.0</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="2" t="s">
+    </row>
+    <row r="77" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A77" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="3">
+        <v>45234</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B76" s="3">
-        <v>45234.0</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="2" t="s">
+    <row r="78" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A78" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" s="3">
+        <v>45234</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B77" s="3">
-        <v>45234.0</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="2" t="s">
+    <row r="79" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A79" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" s="3">
+        <v>45234</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A80" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3">
+        <v>45235</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B78" s="3">
-        <v>45235.0</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="2" t="s">
+    <row r="81" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A81" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" s="3">
+        <v>45235</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B79" s="3">
-        <v>45235.0</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" s="2" t="s">
+    <row r="82" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A82" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="2" t="s">
+      <c r="B82" s="3">
+        <v>45235</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="3">
-        <v>45235.0</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="2" t="s">
+    </row>
+    <row r="83" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A83" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83" s="3">
+        <v>45236</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B81" s="3">
-        <v>45236.0</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D81" s="2" t="s">
+    <row r="84" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A84" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="2" t="s">
+      <c r="B84" s="3">
+        <v>45236</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B82" s="3">
-        <v>45236.0</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" s="2" t="s">
+    </row>
+    <row r="85" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A85" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="3">
+        <v>45236</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B83" s="3">
-        <v>45236.0</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="2" t="s">
+    <row r="86" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A86" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" s="3">
+        <v>45236</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" s="3">
+        <v>45237</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B84" s="3">
-        <v>45237.0</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="2" t="s">
+    <row r="88" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="3">
+        <v>45237</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B85" s="3">
-        <v>45237.0</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="2" t="s">
+    <row r="89" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A89" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="3">
+        <v>45237</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="2" t="s">
+    <row r="90" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A90" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90" s="3">
+        <v>45237</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A91" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" s="3">
+        <v>45237</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B86" s="3">
-        <v>45237.0</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D86" s="2" t="s">
+    </row>
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B87" s="3">
-        <v>45237.0</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" s="2" t="s">
+      <c r="B92" s="7">
+        <v>45247</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="6" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>